<commit_message>
ben/alpha-16: clean up artifact functionaliity
</commit_message>
<xml_diff>
--- a/Plans/Cards_and_Classes.xlsx
+++ b/Plans/Cards_and_Classes.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\Desktop\Card Game\Unity-Card-Game-2020\Plans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Card Game 2020\Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CF890E-CC02-4A76-835B-66727DE4CDDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -1103,7 +1104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1431,28 +1432,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="84.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="99.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="99.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -1463,7 +1464,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -1489,7 +1490,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1518,7 +1519,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1564,7 +1565,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -1627,12 +1628,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1652,7 +1653,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1678,7 +1679,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>89</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -1709,7 +1710,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>122</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>123</v>
       </c>
@@ -1734,7 +1735,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>124</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>125</v>
       </c>
@@ -1768,7 +1769,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>126</v>
       </c>
@@ -1785,7 +1786,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>41</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>7</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>109</v>
       </c>
@@ -1824,7 +1825,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>115</v>
       </c>
@@ -1835,12 +1836,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>101</v>
       </c>
@@ -1854,7 +1855,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>9</v>
       </c>
@@ -1865,7 +1866,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>8</v>
       </c>
@@ -1876,7 +1877,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>2</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>5</v>
       </c>
@@ -1898,7 +1899,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>31</v>
       </c>
@@ -1906,7 +1907,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>6</v>
       </c>
@@ -1914,12 +1915,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D41">
         <v>4</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D42">
         <v>10</v>
       </c>
@@ -1935,7 +1936,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>203</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
         <v>102</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>119</v>
       </c>
@@ -1974,7 +1975,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>40</v>
       </c>
@@ -1982,7 +1983,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>110</v>
       </c>
@@ -1993,12 +1994,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H49" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
         <v>103</v>
       </c>
@@ -2012,7 +2013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>39</v>
       </c>
@@ -2023,7 +2024,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D58">
         <v>0</v>
       </c>
@@ -2031,7 +2032,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>202</v>
       </c>
@@ -2042,7 +2043,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
         <v>105</v>
       </c>
@@ -2050,22 +2051,22 @@
         <v>135</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H62" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H63" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H64" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D65">
         <v>5</v>
       </c>
@@ -2073,12 +2074,12 @@
         <v>198</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H66" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
         <v>104</v>
       </c>
@@ -2092,7 +2093,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D69">
         <v>2</v>
       </c>
@@ -2106,7 +2107,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D70">
         <v>5</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D71">
         <v>4</v>
       </c>
@@ -2125,17 +2126,17 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H72" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H73" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
         <v>126</v>
       </c>
@@ -2146,7 +2147,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D76">
         <v>4</v>
       </c>
@@ -2154,12 +2155,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H77" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>88</v>
       </c>
@@ -2170,12 +2171,12 @@
         <v>132</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H79" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D80">
         <v>10</v>
       </c>
@@ -2186,17 +2187,17 @@
         <v>139</v>
       </c>
     </row>
-    <row r="81" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H81" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="82" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H82" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="85" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C85" t="s">
         <v>354</v>
       </c>
@@ -2213,12 +2214,12 @@
         <v>356</v>
       </c>
     </row>
-    <row r="94" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C94" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
         <v>6</v>
       </c>
@@ -2230,21 +2231,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>149</v>
       </c>
@@ -2252,12 +2253,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>151</v>
       </c>
@@ -2265,7 +2266,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>152</v>
       </c>
@@ -2273,7 +2274,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>153</v>
       </c>
@@ -2281,7 +2282,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>154</v>
       </c>
@@ -2289,157 +2290,157 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>189</v>
       </c>
@@ -2450,29 +2451,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="122" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>52</v>
       </c>
@@ -2492,7 +2493,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>45</v>
       </c>
@@ -2509,7 +2510,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>43</v>
       </c>
@@ -2526,7 +2527,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>44</v>
       </c>
@@ -2540,7 +2541,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>46</v>
       </c>
@@ -2554,7 +2555,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>49</v>
       </c>
@@ -2568,7 +2569,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>50</v>
       </c>
@@ -2582,7 +2583,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>75</v>
       </c>
@@ -2596,12 +2597,12 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -2615,7 +2616,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>64</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>74</v>
       </c>
@@ -2637,7 +2638,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="7:8" x14ac:dyDescent="0.25">
       <c r="G23" t="s">
         <v>229</v>
       </c>
@@ -2645,77 +2646,77 @@
         <v>224</v>
       </c>
     </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H24" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="31" spans="7:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="7:8" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H33" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H34" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H35" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H38" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H39" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H40" t="s">
         <v>238</v>
       </c>
@@ -2726,28 +2727,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" style="2"/>
-    <col min="9" max="9" width="64.6640625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="10.77734375" style="2"/>
+    <col min="1" max="1" width="60.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="2"/>
+    <col min="9" max="9" width="64.7109375" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="10.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>247</v>
       </c>
@@ -2755,7 +2756,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>248</v>
       </c>
@@ -2763,57 +2764,57 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D3" s="2" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E12" s="4" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>329</v>
       </c>
@@ -2845,7 +2846,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" s="2" t="s">
         <v>274</v>
       </c>
@@ -2859,7 +2860,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
         <v>259</v>
       </c>
@@ -2873,7 +2874,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D16" s="2" t="s">
         <v>272</v>
       </c>
@@ -2887,7 +2888,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D17" s="2" t="s">
         <v>252</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
         <v>265</v>
       </c>
@@ -2915,7 +2916,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D19" s="2" t="s">
         <v>297</v>
       </c>
@@ -2932,7 +2933,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D20" s="2" t="s">
         <v>279</v>
       </c>
@@ -2949,11 +2950,11 @@
         <v>278</v>
       </c>
     </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D22" s="2" t="s">
         <v>319</v>
       </c>
@@ -2967,7 +2968,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D23" s="2" t="s">
         <v>345</v>
       </c>
@@ -2981,7 +2982,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
         <v>321</v>
       </c>
@@ -2995,7 +2996,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D25" s="2" t="s">
         <v>322</v>
       </c>
@@ -3009,7 +3010,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D26" s="2" t="s">
         <v>320</v>
       </c>
@@ -3023,7 +3024,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D27" s="2" t="s">
         <v>324</v>
       </c>
@@ -3037,7 +3038,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D28" s="2" t="s">
         <v>318</v>
       </c>
@@ -3051,11 +3052,11 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E30" s="4" t="s">
         <v>256</v>
       </c>
@@ -3063,7 +3064,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E31" s="4" t="s">
         <v>264</v>
       </c>
@@ -3071,7 +3072,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:9" x14ac:dyDescent="0.25">
       <c r="E32" s="4" t="s">
         <v>257</v>
       </c>
@@ -3079,7 +3080,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E33" s="4" t="s">
         <v>327</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E34" s="4" t="s">
         <v>263</v>
       </c>
@@ -3095,7 +3096,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D35" s="2" t="s">
         <v>260</v>
       </c>
@@ -3112,7 +3113,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E36" s="4" t="s">
         <v>328</v>
       </c>
@@ -3120,7 +3121,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D38" s="2" t="s">
         <v>338</v>
       </c>
@@ -3134,37 +3135,37 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H39" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H40" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H41" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H42" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H43" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:8" x14ac:dyDescent="0.25">
       <c r="H44" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D48" s="2" t="s">
         <v>302</v>
       </c>
@@ -3175,7 +3176,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D49" s="2" t="s">
         <v>298</v>
       </c>
@@ -3183,7 +3184,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C50" s="2" t="s">
         <v>295</v>
       </c>
@@ -3197,7 +3198,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D52" s="2" t="s">
         <v>351</v>
       </c>
@@ -3214,7 +3215,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E53" s="4" t="s">
         <v>284</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E54" s="4" t="s">
         <v>285</v>
       </c>
@@ -3230,7 +3231,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D55" s="2" t="s">
         <v>273</v>
       </c>
@@ -3241,7 +3242,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D56" s="2" t="s">
         <v>268</v>
       </c>
@@ -3252,7 +3253,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D57" s="2" t="s">
         <v>267</v>
       </c>
@@ -3263,7 +3264,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D58" s="2" t="s">
         <v>269</v>
       </c>
@@ -3274,7 +3275,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D59" s="2" t="s">
         <v>326</v>
       </c>
@@ -3285,7 +3286,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D61" s="2" t="s">
         <v>312</v>
       </c>
@@ -3296,7 +3297,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D62" s="2" t="s">
         <v>280</v>
       </c>
@@ -3307,7 +3308,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D63" s="2" t="s">
         <v>289</v>
       </c>
@@ -3318,7 +3319,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="64" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
       <c r="D64" s="2" t="s">
         <v>291</v>
       </c>
@@ -3326,7 +3327,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="68" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D68" s="2" t="s">
         <v>317</v>
       </c>
@@ -3337,7 +3338,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="71" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D71" s="2" t="s">
         <v>253</v>
       </c>
@@ -3348,17 +3349,17 @@
         <v>332</v>
       </c>
     </row>
-    <row r="72" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D72" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="73" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D73" s="2" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="76" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D76" s="2" t="s">
         <v>308</v>
       </c>
@@ -3366,7 +3367,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="77" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D77" s="2" t="s">
         <v>309</v>
       </c>
@@ -3374,7 +3375,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="78" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D78" s="2" t="s">
         <v>310</v>
       </c>
@@ -3385,7 +3386,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="79" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D79" s="2" t="s">
         <v>340</v>
       </c>
@@ -3393,7 +3394,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="82" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D82" s="2" t="s">
         <v>334</v>
       </c>
@@ -3401,7 +3402,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="83" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D83" s="2" t="s">
         <v>335</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D84" s="2" t="s">
         <v>336</v>
       </c>
@@ -3420,7 +3421,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="85" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D85" s="2" t="s">
         <v>339</v>
       </c>
@@ -3431,7 +3432,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="86" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D86" s="2" t="s">
         <v>341</v>
       </c>
@@ -3442,7 +3443,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="93" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D93" s="2" t="s">
         <v>349</v>
       </c>
@@ -3459,7 +3460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D94" s="2" t="s">
         <v>353</v>
       </c>
@@ -3476,7 +3477,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E95" s="4" t="s">
         <v>325</v>
       </c>
@@ -3490,7 +3491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D96" s="2" t="s">
         <v>352</v>
       </c>
@@ -3507,7 +3508,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="5:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E97" s="4" t="s">
         <v>348</v>
       </c>

</xml_diff>

<commit_message>
ben/alpha-16: object deep copying, card rewards, loading from battle to battle with preserved data
</commit_message>
<xml_diff>
--- a/Plans/Cards_and_Classes.xlsx
+++ b/Plans/Cards_and_Classes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\Card Game 2020\Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CF890E-CC02-4A76-835B-66727DE4CDDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{834A6FFE-6A93-4265-B9F9-C9B3441F384A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Characters" sheetId="1" r:id="rId1"/>
@@ -1435,8 +1435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,8 +2730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48:H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>